<commit_message>
added test cases and shell scripting to install dependencies and run application
</commit_message>
<xml_diff>
--- a/docs/Test_cases.xlsx
+++ b/docs/Test_cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RobyV\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RobyV\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA410BA5-46D5-44AD-AF0C-2CF25CB3C807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188FF3A2-950C-440F-99CE-75FEBA586D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="10420" xr2:uid="{88A1C4C7-2A3C-4972-AC32-97B4DE5DA657}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{88A1C4C7-2A3C-4972-AC32-97B4DE5DA657}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
   <si>
     <t>Test scenario</t>
   </si>
@@ -106,22 +106,184 @@
     <t>Select products</t>
   </si>
   <si>
-    <t>Select coconut and maggi from the list</t>
-  </si>
-  <si>
-    <t>Coconut and maggi shoul be selectable</t>
-  </si>
-  <si>
-    <t>Coconut and maggi are selectable</t>
-  </si>
-  <si>
     <t>Press enter and enter the quantities and view cart</t>
   </si>
   <si>
-    <t>Items should be in the cart</t>
-  </si>
-  <si>
-    <t>Items with total price are in the cart</t>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>User Customer should have been selected from main menu</t>
+  </si>
+  <si>
+    <t>Select 'Delete product/products from cart option in Customer menu'</t>
+  </si>
+  <si>
+    <t>Coconut and maggi are selectable. Both prompts appeared in the console</t>
+  </si>
+  <si>
+    <t>Coconut and maggi shoul be selectable.                                                             'How much Coconut quantity do you need?' and 'How much Maggi quantity do you need?' prompts should be asked in the console following one another</t>
+  </si>
+  <si>
+    <t>Items should be in the cart with item name quantity , unit price, line total and subtotal.</t>
+  </si>
+  <si>
+    <t>Items with name, quantity, unit price, line total and sub total are in the cart.</t>
+  </si>
+  <si>
+    <t>Delete products</t>
+  </si>
+  <si>
+    <t>Product lists should be visible in the console to select the products for  deletetion from cart</t>
+  </si>
+  <si>
+    <t>Products are visible with name and selectable checkbox</t>
+  </si>
+  <si>
+    <t>Select Coconut from the menu and hit enter button</t>
+  </si>
+  <si>
+    <t>"Do you want to remove all of the product line?" prompt should be displayed</t>
+  </si>
+  <si>
+    <t>"Do you want to remove all of the product line?" prompt displayed</t>
+  </si>
+  <si>
+    <t>Enter Y or y and then View cart</t>
+  </si>
+  <si>
+    <t>Coconut line should have been removed from the cart</t>
+  </si>
+  <si>
+    <t>Coconut line completely removed</t>
+  </si>
+  <si>
+    <t>Select coconut and maggi from the list(hit space bar to select)</t>
+  </si>
+  <si>
+    <t>Repeat step 7 and select Maggi from the item list and hit enter and select n for the prompt. Then enter the quantity 1 to delete. Then select 'View cart' from customer menu.</t>
+  </si>
+  <si>
+    <t>Maggi quantity should have been reduced to 2.</t>
+  </si>
+  <si>
+    <t>Cart contains 2 quantity of Maggi</t>
+  </si>
+  <si>
+    <t>Proceed to checkout</t>
+  </si>
+  <si>
+    <t>Select "Proceed to checkout" from Customer menu and select Cash</t>
+  </si>
+  <si>
+    <t>The total amount to be paid should be displayed , i.e $2</t>
+  </si>
+  <si>
+    <t>$2 displayed on the console</t>
+  </si>
+  <si>
+    <t>Run application in full screen mode for better experience</t>
+  </si>
+  <si>
+    <t>Enter 3 on the console</t>
+  </si>
+  <si>
+    <t>A message of your balance $1 should be displayed  and 'Thank you for your payment' message should be displayed.</t>
+  </si>
+  <si>
+    <t>Here is your balance - $1.0' is displayed. Also 'Thank you for shopping, see you again' message is displayed</t>
+  </si>
+  <si>
+    <t>Select 'Add product' from Customer menu and add 3 quantitis of Maggi and select 'Proceed to checkout'.Then selct card option for payment. Enter card no starting with 5 then 15 more random numbers.</t>
+  </si>
+  <si>
+    <t>Message 'card type unknown, try doing payment again' and 'Wrong card type detected, please try again' displayed. And also 'Please enter card no' message is displayed</t>
+  </si>
+  <si>
+    <t>Enter 16 digit random card numbers starting with 4. Also 'Please enter the expiry date in mm/yy should be displayed'</t>
+  </si>
+  <si>
+    <t>Message 'card type unknown, try doing payment again' and 'Wrong card type detected, please try again' should be displayed. Another prompt to enter the card number again should be also displayed.</t>
+  </si>
+  <si>
+    <t>Visa type card is displayed in console. 'Please enter the expiry date in mm/yy should be displayed'</t>
+  </si>
+  <si>
+    <t>Visa and the entered card number is displayed back. 'Please enter the expiry date in mm/yy is  displayed'</t>
+  </si>
+  <si>
+    <t>Please enter the expity date in mm/yy format and 3 digit CVV number(both random)</t>
+  </si>
+  <si>
+    <t>Thank you for your payment, see you next time ' should be displayed</t>
+  </si>
+  <si>
+    <t>Thank you for your payment, see you next time' is displayed</t>
+  </si>
+  <si>
+    <t>Proceed to checkout- card type selection</t>
+  </si>
+  <si>
+    <t>Proceed to checkout - card type selection</t>
+  </si>
+  <si>
+    <t>Select 'Add product' from Customer menu and add 3 quantitis of Almonds and select 'Proceed to checkout'.Then selct card option for payment. Enter card no starting with 55 then 14 more random numbers.</t>
+  </si>
+  <si>
+    <t>Card type should be displayed as MasterCard</t>
+  </si>
+  <si>
+    <t>MastedCard displayed</t>
+  </si>
+  <si>
+    <t>View Cart</t>
+  </si>
+  <si>
+    <t>Select 'Add product' then select 'Apple' and 'Orange' from the menu list. Hit enter. Enter the quantities os Apple and Orange to 2 and 4 respectively. Then select 'View Cart' from Customer menu</t>
+  </si>
+  <si>
+    <t>Table view of cart should be displayed with line for Apple contianing Quantity -2 , Unit price 1.0 and line total 2.0. Another line for Orange with quantity 4, unit price 1.0 and line total 4.0. and then subtotal of 6.0</t>
+  </si>
+  <si>
+    <t>Cart table displayed with line for Apple contianing Quantity -2 , Unit price 1.0 and line total 2.0. Another line for Orange with quantity 4, unit price 1.0 and line total 4.0. and then subtotal of 6.0</t>
+  </si>
+  <si>
+    <t>Owner should be selected from main menu, by completing the checkout and by selecting Exit to main menu from customer menu</t>
+  </si>
+  <si>
+    <t>Change the price of a product</t>
+  </si>
+  <si>
+    <t>Select 'Change the price of a product' from Owner menu. Then select Coconut and Milk from the list,hit enter and enter the new price for Coconut and Milk as 7 and 22. Then select Display products.</t>
+  </si>
+  <si>
+    <t>Add a new product</t>
+  </si>
+  <si>
+    <t>Enter Lolliesand unit price of 3.0. and also enter the stock available as 5. Now 'enter display products' from the owner menu.</t>
+  </si>
+  <si>
+    <t>Delete an existing product</t>
+  </si>
+  <si>
+    <t>Select 'Delete an existing product from the Owner menu'. Select 'Jam' from the menu list and hit enter.Then selct Display products from the Owner menu.</t>
+  </si>
+  <si>
+    <t>Product Jam shoul be deleted from the table and JSON file(/src/data/products.json)</t>
+  </si>
+  <si>
+    <t>The product table should contain product 'Lollies' unit price of 3.0 and stock availability of 5. The product must be also present in JSON file(/src/data/products.json)</t>
+  </si>
+  <si>
+    <t>Unit price of coconut and milk should have been changed to 7.0 and 22.0 respectively in table and in JSON file(/src/data/products.json)</t>
+  </si>
+  <si>
+    <t>Unit price of coconut and milk changed to 7.0 and 22.0 respectively.Price changed in JSON file also in path (/src/data/products.json)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> product table contains product 'Lollies' unit price of 3.0 and stock availability of 5. Product Lollies added to JSON file in path (/src/data/products.json)</t>
+  </si>
+  <si>
+    <t>Product Jam is deleted from the table displayed and also from the products JSON file from path (/src/data/products.json).</t>
   </si>
 </sst>
 </file>
@@ -165,10 +327,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -485,158 +650,502 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EE956B-00B7-47B3-B3AC-AAC96AE83B73}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F7"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" customWidth="1"/>
-    <col min="4" max="4" width="60.81640625" customWidth="1"/>
-    <col min="5" max="5" width="33.54296875" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>